<commit_message>
Final addition of sprint 3 documentation
</commit_message>
<xml_diff>
--- a/CodeMetrics.xlsx
+++ b/CodeMetrics.xlsx
@@ -299,6 +299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -375,7 +376,42 @@
         <v>0.0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>44494.0</v>
+      </c>
+      <c r="B3" s="1">
+        <v>83.0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1676.0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>231.0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>9061.0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>2359.0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>422.0</v>
+      </c>
+    </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>